<commit_message>
Created example classrooms to fit large amount of students
</commit_message>
<xml_diff>
--- a/large_amount_of_rooms.xlsx
+++ b/large_amount_of_rooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C790B7C-E3CB-4A1E-9BBB-784173C1A660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A75B683-F897-48D4-96EC-9DD358B06326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="4395" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="235">
   <si>
     <t>Color Code</t>
   </si>
@@ -854,9 +854,6 @@
     <t>11-535</t>
   </si>
   <si>
-    <t>11-536</t>
-  </si>
-  <si>
     <t>11-537</t>
   </si>
   <si>
@@ -875,16 +872,16 @@
     <t>11-324C Computer Lab</t>
   </si>
   <si>
-    <t>11-325C Computer Lab</t>
-  </si>
-  <si>
-    <t>11-625C Computer Lab</t>
-  </si>
-  <si>
     <t>11-5312</t>
   </si>
   <si>
     <t>11-329C Computer Lab</t>
+  </si>
+  <si>
+    <t>11-5319</t>
+  </si>
+  <si>
+    <t>11-421</t>
   </si>
 </sst>
 </file>
@@ -1901,28 +1898,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1946,29 +1946,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2964,11 +2961,11 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" s="165" t="s">
+      <c r="A2" s="144" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
     </row>
     <row r="3" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="140" t="s">
@@ -2978,11 +2975,11 @@
       <c r="C3" s="140"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="166" t="s">
+      <c r="A4" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="166"/>
-      <c r="C4" s="166"/>
+      <c r="B4" s="145"/>
+      <c r="C4" s="145"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
@@ -2993,48 +2990,48 @@
       </c>
       <c r="B6" s="142"/>
       <c r="C6" s="142"/>
-      <c r="D6" s="151" t="s">
+      <c r="D6" s="146" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="46"/>
-      <c r="F6" s="162" t="s">
+      <c r="F6" s="147" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="160" t="s">
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
+      <c r="I6" s="148" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="47"/>
-      <c r="K6" s="162" t="s">
+      <c r="K6" s="147" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="162"/>
-      <c r="M6" s="162"/>
-      <c r="N6" s="160" t="s">
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="148" t="s">
         <v>5</v>
       </c>
       <c r="O6" s="48"/>
-      <c r="P6" s="162" t="s">
+      <c r="P6" s="147" t="s">
         <v>74</v>
       </c>
-      <c r="Q6" s="162"/>
-      <c r="R6" s="162"/>
-      <c r="S6" s="160" t="s">
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="148" t="s">
         <v>5</v>
       </c>
-      <c r="T6" s="161" t="s">
+      <c r="T6" s="149" t="s">
         <v>75</v>
       </c>
-      <c r="V6" s="162" t="s">
+      <c r="V6" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="W6" s="162"/>
-      <c r="X6" s="162"/>
-      <c r="Y6" s="163" t="s">
+      <c r="W6" s="147"/>
+      <c r="X6" s="147"/>
+      <c r="Y6" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="Z6" s="164" t="s">
+      <c r="Z6" s="151" t="s">
         <v>75</v>
       </c>
       <c r="AB6" s="142" t="s">
@@ -3042,7 +3039,7 @@
       </c>
       <c r="AC6" s="142"/>
       <c r="AD6" s="142"/>
-      <c r="AE6" s="151" t="s">
+      <c r="AE6" s="146" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3050,79 +3047,79 @@
       <c r="A7" s="142"/>
       <c r="B7" s="142"/>
       <c r="C7" s="142"/>
-      <c r="D7" s="151"/>
+      <c r="D7" s="146"/>
       <c r="E7" s="46"/>
-      <c r="F7" s="162"/>
-      <c r="G7" s="162"/>
-      <c r="H7" s="162"/>
-      <c r="I7" s="160"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="148"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="162"/>
-      <c r="L7" s="162"/>
-      <c r="M7" s="162"/>
-      <c r="N7" s="160"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="148"/>
       <c r="O7" s="48"/>
-      <c r="P7" s="162"/>
-      <c r="Q7" s="162"/>
-      <c r="R7" s="162"/>
-      <c r="S7" s="160"/>
-      <c r="T7" s="161"/>
-      <c r="V7" s="162"/>
-      <c r="W7" s="162"/>
-      <c r="X7" s="162"/>
-      <c r="Y7" s="163"/>
-      <c r="Z7" s="164"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="147"/>
+      <c r="S7" s="148"/>
+      <c r="T7" s="149"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="147"/>
+      <c r="X7" s="147"/>
+      <c r="Y7" s="150"/>
+      <c r="Z7" s="151"/>
       <c r="AB7" s="142"/>
       <c r="AC7" s="142"/>
       <c r="AD7" s="142"/>
-      <c r="AE7" s="151"/>
+      <c r="AE7" s="146"/>
     </row>
     <row r="8" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="142"/>
       <c r="B8" s="142"/>
       <c r="C8" s="142"/>
-      <c r="D8" s="151"/>
+      <c r="D8" s="146"/>
       <c r="E8" s="46"/>
-      <c r="F8" s="162"/>
-      <c r="G8" s="162"/>
-      <c r="H8" s="162"/>
-      <c r="I8" s="160"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="148"/>
       <c r="J8" s="47"/>
-      <c r="K8" s="162"/>
-      <c r="L8" s="162"/>
-      <c r="M8" s="162"/>
-      <c r="N8" s="160"/>
+      <c r="K8" s="147"/>
+      <c r="L8" s="147"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="148"/>
       <c r="O8" s="48"/>
-      <c r="P8" s="162"/>
-      <c r="Q8" s="162"/>
-      <c r="R8" s="162"/>
-      <c r="S8" s="160"/>
-      <c r="T8" s="161"/>
-      <c r="V8" s="162"/>
-      <c r="W8" s="162"/>
-      <c r="X8" s="162"/>
-      <c r="Y8" s="163"/>
-      <c r="Z8" s="164"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="148"/>
+      <c r="T8" s="149"/>
+      <c r="V8" s="147"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="147"/>
+      <c r="Y8" s="150"/>
+      <c r="Z8" s="151"/>
       <c r="AB8" s="142"/>
       <c r="AC8" s="142"/>
       <c r="AD8" s="142"/>
-      <c r="AE8" s="151"/>
+      <c r="AE8" s="146"/>
     </row>
     <row r="9" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="146" t="s">
+      <c r="A9" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="152" t="s">
+      <c r="B9" s="153" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="153" t="s">
+      <c r="C9" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="154">
+      <c r="D9" s="155">
         <v>21</v>
       </c>
       <c r="E9" s="50"/>
-      <c r="F9" s="155" t="s">
+      <c r="F9" s="156" t="s">
         <v>78</v>
       </c>
       <c r="G9" s="51" t="s">
@@ -3148,7 +3145,7 @@
         <v>21</v>
       </c>
       <c r="O9" s="55"/>
-      <c r="P9" s="156" t="s">
+      <c r="P9" s="157" t="s">
         <v>78</v>
       </c>
       <c r="Q9" s="51" t="s">
@@ -3184,12 +3181,12 @@
       </c>
     </row>
     <row r="10" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="146"/>
-      <c r="B10" s="152"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="154"/>
+      <c r="A10" s="152"/>
+      <c r="B10" s="153"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="50"/>
-      <c r="F10" s="155"/>
+      <c r="F10" s="156"/>
       <c r="G10" s="7" t="s">
         <v>89</v>
       </c>
@@ -3211,7 +3208,7 @@
         <v>21</v>
       </c>
       <c r="O10" s="55"/>
-      <c r="P10" s="156"/>
+      <c r="P10" s="157"/>
       <c r="Q10" s="7" t="s">
         <v>93</v>
       </c>
@@ -3247,25 +3244,25 @@
       </c>
     </row>
     <row r="11" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="146"/>
-      <c r="B11" s="157" t="s">
+      <c r="A11" s="152"/>
+      <c r="B11" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="158" t="s">
+      <c r="C11" s="159" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="144">
+      <c r="D11" s="160">
         <v>14</v>
       </c>
       <c r="E11" s="73"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="159" t="s">
+      <c r="F11" s="156"/>
+      <c r="G11" s="161" t="s">
         <v>101</v>
       </c>
-      <c r="H11" s="158" t="s">
+      <c r="H11" s="159" t="s">
         <v>102</v>
       </c>
-      <c r="I11" s="144">
+      <c r="I11" s="160">
         <v>21</v>
       </c>
       <c r="J11" s="54"/>
@@ -3280,7 +3277,7 @@
         <v>15</v>
       </c>
       <c r="O11" s="55"/>
-      <c r="P11" s="156"/>
+      <c r="P11" s="157"/>
       <c r="Q11" s="7" t="s">
         <v>105</v>
       </c>
@@ -3318,15 +3315,15 @@
       </c>
     </row>
     <row r="12" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="146"/>
-      <c r="B12" s="157"/>
-      <c r="C12" s="158"/>
-      <c r="D12" s="144"/>
+      <c r="A12" s="152"/>
+      <c r="B12" s="158"/>
+      <c r="C12" s="159"/>
+      <c r="D12" s="160"/>
       <c r="E12" s="73"/>
-      <c r="F12" s="155"/>
-      <c r="G12" s="159"/>
-      <c r="H12" s="158"/>
-      <c r="I12" s="144"/>
+      <c r="F12" s="156"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="159"/>
+      <c r="I12" s="160"/>
       <c r="J12" s="54"/>
       <c r="K12" s="138"/>
       <c r="L12" s="7" t="s">
@@ -3339,7 +3336,7 @@
         <v>50</v>
       </c>
       <c r="O12" s="55"/>
-      <c r="P12" s="156"/>
+      <c r="P12" s="157"/>
       <c r="Q12" s="7" t="s">
         <v>114</v>
       </c>
@@ -3378,7 +3375,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="146"/>
+      <c r="A13" s="152"/>
       <c r="B13" s="72" t="s">
         <v>120</v>
       </c>
@@ -3389,7 +3386,7 @@
         <v>21</v>
       </c>
       <c r="E13" s="73"/>
-      <c r="F13" s="155"/>
+      <c r="F13" s="156"/>
       <c r="G13" s="7" t="s">
         <v>122</v>
       </c>
@@ -3410,7 +3407,7 @@
         <v>107</v>
       </c>
       <c r="O13" s="55"/>
-      <c r="P13" s="156"/>
+      <c r="P13" s="157"/>
       <c r="Q13" s="7" t="s">
         <v>125</v>
       </c>
@@ -3435,7 +3432,7 @@
       </c>
       <c r="Z13" s="82"/>
       <c r="AA13" s="83"/>
-      <c r="AB13" s="145" t="s">
+      <c r="AB13" s="162" t="s">
         <v>18</v>
       </c>
       <c r="AC13" s="51" t="s">
@@ -3449,7 +3446,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="146"/>
+      <c r="A14" s="152"/>
       <c r="B14" s="55"/>
       <c r="C14" s="86" t="s">
         <v>131</v>
@@ -3459,7 +3456,7 @@
         <v>56</v>
       </c>
       <c r="E14" s="88"/>
-      <c r="F14" s="155"/>
+      <c r="F14" s="156"/>
       <c r="G14" s="89"/>
       <c r="H14" s="90" t="s">
         <v>132</v>
@@ -3482,7 +3479,7 @@
         <v>15</v>
       </c>
       <c r="O14" s="55"/>
-      <c r="P14" s="156"/>
+      <c r="P14" s="157"/>
       <c r="Q14" s="80"/>
       <c r="R14" s="76" t="s">
         <v>135</v>
@@ -3507,7 +3504,7 @@
       </c>
       <c r="Z14" s="96"/>
       <c r="AA14" s="59"/>
-      <c r="AB14" s="145"/>
+      <c r="AB14" s="162"/>
       <c r="AC14" s="51" t="s">
         <v>138</v>
       </c>
@@ -3519,7 +3516,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="146" t="s">
+      <c r="A15" s="152" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="98" t="s">
@@ -3532,7 +3529,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="50"/>
-      <c r="F15" s="147" t="s">
+      <c r="F15" s="163" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -3583,7 +3580,7 @@
         <v>18</v>
       </c>
       <c r="Z15" s="100"/>
-      <c r="AB15" s="145"/>
+      <c r="AB15" s="162"/>
       <c r="AC15" s="51" t="s">
         <v>151</v>
       </c>
@@ -3595,7 +3592,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="146"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="81" t="s">
         <v>153</v>
       </c>
@@ -3606,7 +3603,7 @@
         <v>21</v>
       </c>
       <c r="E16" s="50"/>
-      <c r="F16" s="147"/>
+      <c r="F16" s="163"/>
       <c r="G16" s="7" t="s">
         <v>155</v>
       </c>
@@ -3656,7 +3653,7 @@
         <v>164</v>
       </c>
       <c r="AA16" s="59"/>
-      <c r="AB16" s="145"/>
+      <c r="AB16" s="162"/>
       <c r="AC16" s="76"/>
       <c r="AD16" s="77" t="s">
         <v>165</v>
@@ -3667,7 +3664,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="146"/>
+      <c r="A17" s="152"/>
       <c r="B17" s="81" t="s">
         <v>166</v>
       </c>
@@ -3678,7 +3675,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="50"/>
-      <c r="F17" s="147"/>
+      <c r="F17" s="163"/>
       <c r="G17" s="16" t="s">
         <v>168</v>
       </c>
@@ -3727,7 +3724,7 @@
         <v>162</v>
       </c>
       <c r="AA17" s="59"/>
-      <c r="AB17" s="148" t="s">
+      <c r="AB17" s="164" t="s">
         <v>26</v>
       </c>
       <c r="AC17" s="51" t="s">
@@ -3741,7 +3738,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="146"/>
+      <c r="A18" s="152"/>
       <c r="B18" s="81" t="s">
         <v>178</v>
       </c>
@@ -3752,7 +3749,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="147"/>
+      <c r="F18" s="163"/>
       <c r="G18" s="89"/>
       <c r="H18" s="90" t="s">
         <v>180</v>
@@ -3762,7 +3759,7 @@
         <v>70</v>
       </c>
       <c r="J18" s="54"/>
-      <c r="K18" s="149" t="s">
+      <c r="K18" s="165" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="92" t="s">
@@ -3800,7 +3797,7 @@
       </c>
       <c r="Z18" s="108"/>
       <c r="AA18" s="109"/>
-      <c r="AB18" s="148"/>
+      <c r="AB18" s="164"/>
       <c r="AC18" s="51" t="s">
         <v>187</v>
       </c>
@@ -3812,7 +3809,7 @@
       </c>
     </row>
     <row r="19" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
+      <c r="A19" s="152"/>
       <c r="B19" s="55"/>
       <c r="C19" s="86" t="s">
         <v>189</v>
@@ -3835,7 +3832,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="54"/>
-      <c r="K19" s="149"/>
+      <c r="K19" s="165"/>
       <c r="L19" s="7" t="s">
         <v>192</v>
       </c>
@@ -3874,7 +3871,7 @@
       </c>
       <c r="Z19" s="96"/>
       <c r="AA19" s="59"/>
-      <c r="AB19" s="148"/>
+      <c r="AB19" s="164"/>
       <c r="AC19" s="76"/>
       <c r="AD19" s="77" t="s">
         <v>199</v>
@@ -3885,7 +3882,7 @@
       </c>
     </row>
     <row r="20" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="150" t="s">
+      <c r="A20" s="166" t="s">
         <v>200</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -3909,7 +3906,7 @@
         <v>39</v>
       </c>
       <c r="J20" s="54"/>
-      <c r="K20" s="149"/>
+      <c r="K20" s="165"/>
       <c r="L20" s="80"/>
       <c r="M20" s="76" t="s">
         <v>205</v>
@@ -3944,7 +3941,7 @@
       <c r="AA20" s="59"/>
     </row>
     <row r="21" spans="1:31" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="150"/>
+      <c r="A21" s="166"/>
       <c r="B21" s="8" t="s">
         <v>209</v>
       </c>
@@ -3997,7 +3994,7 @@
       <c r="AB21" s="115"/>
     </row>
     <row r="22" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="150"/>
+      <c r="A22" s="166"/>
       <c r="B22" s="80"/>
       <c r="C22" s="76" t="s">
         <v>217</v>
@@ -4247,21 +4244,19 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="F6:H8"/>
-    <mergeCell ref="I6:I8"/>
-    <mergeCell ref="K6:M8"/>
-    <mergeCell ref="N6:N8"/>
-    <mergeCell ref="P6:R8"/>
-    <mergeCell ref="S6:S8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="V6:X8"/>
-    <mergeCell ref="Y6:Y8"/>
-    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="AB13:AB16"/>
+    <mergeCell ref="K14:K17"/>
+    <mergeCell ref="V14:V18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="P15:P20"/>
+    <mergeCell ref="AB17:AB19"/>
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="V19:V22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="P21:P22"/>
     <mergeCell ref="AB6:AD8"/>
     <mergeCell ref="AE6:AE8"/>
     <mergeCell ref="A9:A14"/>
@@ -4278,19 +4273,21 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="AB13:AB16"/>
-    <mergeCell ref="K14:K17"/>
-    <mergeCell ref="V14:V18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="P15:P20"/>
-    <mergeCell ref="AB17:AB19"/>
-    <mergeCell ref="K18:K20"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="V19:V22"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="S6:S8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="V6:X8"/>
+    <mergeCell ref="Y6:Y8"/>
+    <mergeCell ref="Z6:Z8"/>
+    <mergeCell ref="F6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="K6:M8"/>
+    <mergeCell ref="N6:N8"/>
+    <mergeCell ref="P6:R8"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C8"/>
+    <mergeCell ref="D6:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4299,10 +4296,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4357,7 +4354,7 @@
         <v>226</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4365,7 +4362,7 @@
         <v>227</v>
       </c>
       <c r="B7">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4378,23 +4375,23 @@
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B11">
         <v>36</v>
@@ -4402,35 +4399,31 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B14">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B15">
-        <v>40</v>
-      </c>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Fixed bug with cohorts not being scheulded
</commit_message>
<xml_diff>
--- a/large_amount_of_rooms.xlsx
+++ b/large_amount_of_rooms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conla\PycharmProjects\2023-01_Team6-Conlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A75B683-F897-48D4-96EC-9DD358B06326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16802DB3-5A02-4571-B43E-F444E5510DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1665" yWindow="4395" windowWidth="21600" windowHeight="10140" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="236">
   <si>
     <t>Color Code</t>
   </si>
@@ -852,6 +852,9 @@
   </si>
   <si>
     <t>11-535</t>
+  </si>
+  <si>
+    <t>11-536</t>
   </si>
   <si>
     <t>11-537</t>
@@ -4296,10 +4299,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ16"/>
+  <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D8" activeCellId="1" sqref="A6:B15 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4354,7 +4357,7 @@
         <v>226</v>
       </c>
       <c r="B6">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4362,7 +4365,7 @@
         <v>227</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4375,18 +4378,18 @@
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B9">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4394,12 +4397,12 @@
         <v>234</v>
       </c>
       <c r="B11">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B12">
         <v>36</v>
@@ -4410,20 +4413,28 @@
         <v>230</v>
       </c>
       <c r="B13">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>